<commit_message>
[excel-pipeline]:ed73624 auto commit ...
</commit_message>
<xml_diff>
--- a/config/excel/Hero.xlsx
+++ b/config/excel/Hero.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E699529-D2A1-4EEC-BE02-734AA28C6560}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hero" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -221,18 +227,72 @@
   <si>
     <t>怪物3</t>
   </si>
+  <si>
+    <t>技能1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>技能4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo版本
+技能1
+普攻攻击</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo版本
+技能2
+战技技能</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo版本
+技能3
+奥义技能</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Demo版本
+技能4
+残响技能</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>int32</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill1</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill2</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill3</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>skill4</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="25">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -244,11 +304,13 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -257,164 +319,25 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="36">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,192 +364,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -649,253 +392,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -911,58 +412,15 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1035,6 +493,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1266,7 +727,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1556,7 +1017,7 @@
           </a:outerShdw>
         </a:effectLst>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1832,7 +1293,7 @@
           <a:miter lim="400000"/>
         </a:ln>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2105,36 +1566,37 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:Q13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:U13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="T8" sqref="T8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="14.35" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.35" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.375" style="1" customWidth="1"/>
     <col min="3" max="3" width="8.5" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.35" style="1" customWidth="1"/>
+    <col min="4" max="5" width="17.375" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="27.625" style="1" customWidth="1"/>
     <col min="8" max="9" width="16.25" style="1" customWidth="1"/>
-    <col min="10" max="13" width="9.425" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.15" style="1" customWidth="1"/>
+    <col min="10" max="13" width="9.375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="16.125" style="1" customWidth="1"/>
     <col min="15" max="15" width="16.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.4583333333333" style="1" customWidth="1"/>
+    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="20.125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="6" style="1" customWidth="1"/>
+    <col min="18" max="21" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14" customHeight="1" spans="1:17">
+    <row r="1" spans="1:21" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2155,7 +1617,7 @@
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
     </row>
-    <row r="2" ht="121" customHeight="1" spans="1:17">
+    <row r="2" spans="1:21" ht="120.95" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -2197,8 +1659,20 @@
       </c>
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
+      <c r="R2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:17">
+    <row r="3" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>13</v>
@@ -2240,8 +1714,20 @@
       <c r="Q3" s="5" t="s">
         <v>24</v>
       </c>
+      <c r="R3" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="T3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="U3" s="10" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:17">
+    <row r="4" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>25</v>
@@ -2291,8 +1777,20 @@
       <c r="Q4" s="5" t="s">
         <v>39</v>
       </c>
+      <c r="R4" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="S4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="T4" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="10" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:17">
+    <row r="5" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -2314,8 +1812,12 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
+      <c r="U5" s="10"/>
     </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:17">
+    <row r="6" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>42</v>
@@ -2357,8 +1859,20 @@
       <c r="Q6" s="5" t="s">
         <v>43</v>
       </c>
+      <c r="R6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="T6" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="10" t="s">
+        <v>64</v>
+      </c>
     </row>
-    <row r="7" ht="25" customHeight="1" spans="1:17">
+    <row r="7" spans="1:21" ht="24.95" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="6">
@@ -2407,8 +1921,20 @@
       <c r="Q7" s="6">
         <v>30</v>
       </c>
+      <c r="R7" s="1">
+        <v>101001</v>
+      </c>
+      <c r="S7" s="1">
+        <v>101002</v>
+      </c>
+      <c r="T7" s="1">
+        <v>101003</v>
+      </c>
+      <c r="U7" s="1">
+        <v>101004</v>
+      </c>
     </row>
-    <row r="8" ht="25" customHeight="1" spans="1:17">
+    <row r="8" spans="1:21" ht="24.95" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="6">
@@ -2457,8 +1983,20 @@
       <c r="Q8" s="6">
         <v>50</v>
       </c>
+      <c r="R8" s="1">
+        <v>102001</v>
+      </c>
+      <c r="S8" s="1">
+        <v>102002</v>
+      </c>
+      <c r="T8" s="1">
+        <v>102003</v>
+      </c>
+      <c r="U8" s="1">
+        <v>102004</v>
+      </c>
     </row>
-    <row r="9" ht="16.15" customHeight="1" spans="1:17">
+    <row r="9" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
@@ -2507,8 +2045,20 @@
       <c r="Q9" s="6">
         <v>30</v>
       </c>
+      <c r="R9" s="1">
+        <v>103001</v>
+      </c>
+      <c r="S9" s="1">
+        <v>103002</v>
+      </c>
+      <c r="T9" s="1">
+        <v>103003</v>
+      </c>
+      <c r="U9" s="1">
+        <v>103004</v>
+      </c>
     </row>
-    <row r="10" ht="14" customHeight="1" spans="1:17">
+    <row r="10" spans="1:21" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
@@ -2557,8 +2107,20 @@
       <c r="Q10" s="6">
         <v>50</v>
       </c>
+      <c r="R10" s="1">
+        <v>104001</v>
+      </c>
+      <c r="S10" s="1">
+        <v>104002</v>
+      </c>
+      <c r="T10" s="1">
+        <v>104003</v>
+      </c>
+      <c r="U10" s="1">
+        <v>104004</v>
+      </c>
     </row>
-    <row r="11" s="1" customFormat="1" ht="25" customHeight="1" spans="1:17">
+    <row r="11" spans="1:21" ht="24.95" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6">
@@ -2607,8 +2169,20 @@
       <c r="Q11" s="6">
         <v>-1</v>
       </c>
+      <c r="R11" s="1">
+        <v>105001</v>
+      </c>
+      <c r="S11" s="1">
+        <v>105002</v>
+      </c>
+      <c r="T11" s="1">
+        <v>105003</v>
+      </c>
+      <c r="U11" s="1">
+        <v>105004</v>
+      </c>
     </row>
-    <row r="12" s="1" customFormat="1" ht="16.15" customHeight="1" spans="1:17">
+    <row r="12" spans="1:21" ht="16.149999999999999" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6">
@@ -2657,8 +2231,20 @@
       <c r="Q12" s="6">
         <v>-1</v>
       </c>
+      <c r="R12" s="1">
+        <v>106001</v>
+      </c>
+      <c r="S12" s="1">
+        <v>106002</v>
+      </c>
+      <c r="T12" s="1">
+        <v>106003</v>
+      </c>
+      <c r="U12" s="1">
+        <v>106004</v>
+      </c>
     </row>
-    <row r="13" s="1" customFormat="1" ht="14" customHeight="1" spans="1:17">
+    <row r="13" spans="1:21" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6">
@@ -2707,10 +2293,23 @@
       <c r="Q13" s="6">
         <v>-1</v>
       </c>
+      <c r="R13" s="1">
+        <v>107001</v>
+      </c>
+      <c r="S13" s="1">
+        <v>107002</v>
+      </c>
+      <c r="T13" s="1">
+        <v>107003</v>
+      </c>
+      <c r="U13" s="1">
+        <v>107004</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:0ee4eee commit_msg:增加模型资源列 ...
</commit_message>
<xml_diff>
--- a/config/excel/Hero.xlsx
+++ b/config/excel/Hero.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66056CD1-3C46-4564-9E69-03DD71CB403E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hero" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="74">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -268,18 +274,32 @@
   <si>
     <t>怪物3</t>
   </si>
+  <si>
+    <t>模型资源</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>modelresource</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>模型资源文件名称</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>puluomixiusi</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -291,11 +311,13 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -311,164 +333,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -499,194 +375,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -709,251 +399,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -976,57 +424,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1099,6 +500,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2169,16 +1573,16 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:U13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2186,20 +1590,20 @@
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.25" style="1" customWidth="1"/>
-    <col min="10" max="13" width="9.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.125" style="1" customWidth="1"/>
-    <col min="18" max="21" width="9.25" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="6" style="1"/>
+    <col min="4" max="6" width="17.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.25" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.125" style="1" customWidth="1"/>
+    <col min="19" max="22" width="9.25" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.1" customHeight="1" spans="1:17">
+    <row r="1" spans="1:22" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2219,63 +1623,67 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
-    <row r="2" ht="120.95" customHeight="1" spans="1:21">
+    <row r="2" spans="1:22" ht="120.95" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:21">
+    <row r="3" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -2287,50 +1695,53 @@
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="S3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:21">
+    <row r="4" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
         <v>33</v>
@@ -2342,58 +1753,61 @@
         <v>34</v>
       </c>
       <c r="E4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:21">
+    <row r="5" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
         <v>52</v>
@@ -2415,12 +1829,13 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="10"/>
+      <c r="R5" s="5"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
     </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:21">
+    <row r="6" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
         <v>54</v>
@@ -2432,10 +1847,10 @@
         <v>56</v>
       </c>
       <c r="E6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="G6" s="5" t="s">
         <v>55</v>
@@ -2446,15 +1861,15 @@
       <c r="I6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="5"/>
+      <c r="J6" s="5" t="s">
+        <v>55</v>
+      </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
+      <c r="N6" s="5"/>
+      <c r="O6" s="5" t="s">
         <v>58</v>
-      </c>
-      <c r="O6" s="5" t="s">
-        <v>55</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>55</v>
@@ -2462,7 +1877,7 @@
       <c r="Q6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="5" t="s">
         <v>55</v>
       </c>
       <c r="S6" s="10" t="s">
@@ -2474,8 +1889,11 @@
       <c r="U6" s="10" t="s">
         <v>55</v>
       </c>
+      <c r="V6" s="10" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="7" ht="24.95" customHeight="1" spans="1:21">
+    <row r="7" spans="1:22" ht="24.95" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="6">
@@ -2485,16 +1903,16 @@
         <v>59</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F7" s="6">
+      <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <v>1</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -2511,33 +1929,36 @@
       <c r="M7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="6" t="str">
-        <f t="shared" ref="N7:N13" si="0">J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7</f>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="str">
+        <f t="shared" ref="O7:O13" si="0">K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7</f>
         <v>0,0,0,0</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>1</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>50</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>30</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>101001</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>101002</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>101003</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>101004</v>
       </c>
     </row>
-    <row r="8" ht="24.95" customHeight="1" spans="1:21">
+    <row r="8" spans="1:22" ht="24.95" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="6">
@@ -2547,16 +1968,16 @@
         <v>61</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
       </c>
       <c r="I8" s="6">
         <v>1</v>
@@ -2573,33 +1994,36 @@
       <c r="M8" s="6">
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="str">
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1,1,1,1</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>2</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>80</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>50</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>102001</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>102002</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>102003</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <v>102004</v>
       </c>
     </row>
-    <row r="9" ht="16.15" customHeight="1" spans="1:21">
+    <row r="9" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
@@ -2609,16 +2033,16 @@
         <v>63</v>
       </c>
       <c r="E9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F9" s="3">
+      <c r="G9" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>3</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2</v>
       </c>
       <c r="I9" s="3">
         <v>2</v>
@@ -2635,33 +2059,36 @@
       <c r="M9" s="3">
         <v>2</v>
       </c>
-      <c r="N9" s="6" t="str">
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>2,2,2,2</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>3</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>50</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>30</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>103001</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>103002</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>103003</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V9" s="1">
         <v>103004</v>
       </c>
     </row>
-    <row r="10" ht="14.1" customHeight="1" spans="1:21">
+    <row r="10" spans="1:22" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
@@ -2671,16 +2098,16 @@
         <v>64</v>
       </c>
       <c r="E10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3</v>
       </c>
       <c r="I10" s="3">
         <v>3</v>
@@ -2697,33 +2124,36 @@
       <c r="M10" s="3">
         <v>3</v>
       </c>
-      <c r="N10" s="6" t="str">
+      <c r="N10" s="3">
+        <v>3</v>
+      </c>
+      <c r="O10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>3,3,3,3</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>4</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>80</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>50</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>104001</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>104002</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>104003</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <v>104004</v>
       </c>
     </row>
-    <row r="11" ht="24.95" customHeight="1" spans="1:21">
+    <row r="11" spans="1:22" ht="24.95" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6">
@@ -2733,19 +2163,19 @@
         <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F11" s="6">
+      <c r="G11" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>-1</v>
       </c>
       <c r="J11" s="6">
         <v>-1</v>
@@ -2759,33 +2189,36 @@
       <c r="M11" s="6">
         <v>-1</v>
       </c>
-      <c r="N11" s="6" t="str">
+      <c r="N11" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <v>5</v>
-      </c>
-      <c r="P11" s="6">
-        <v>-1</v>
       </c>
       <c r="Q11" s="6">
         <v>-1</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S11" s="1">
         <v>105001</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>105002</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>105003</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <v>105004</v>
       </c>
     </row>
-    <row r="12" ht="16.15" customHeight="1" spans="1:21">
+    <row r="12" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6">
@@ -2795,19 +2228,19 @@
         <v>67</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="3">
+      <c r="G12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>2</v>
-      </c>
-      <c r="I12" s="6">
-        <v>-1</v>
       </c>
       <c r="J12" s="6">
         <v>-1</v>
@@ -2821,33 +2254,36 @@
       <c r="M12" s="6">
         <v>-1</v>
       </c>
-      <c r="N12" s="6" t="str">
+      <c r="N12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>6</v>
-      </c>
-      <c r="P12" s="6">
-        <v>-1</v>
       </c>
       <c r="Q12" s="6">
         <v>-1</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S12" s="1">
         <v>106001</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>106002</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>106003</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <v>106004</v>
       </c>
     </row>
-    <row r="13" ht="14.1" customHeight="1" spans="1:21">
+    <row r="13" spans="1:22" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6">
@@ -2857,19 +2293,19 @@
         <v>68</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F13" s="3">
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>3</v>
-      </c>
-      <c r="I13" s="6">
-        <v>-1</v>
       </c>
       <c r="J13" s="6">
         <v>-1</v>
@@ -2883,35 +2319,39 @@
       <c r="M13" s="6">
         <v>-1</v>
       </c>
-      <c r="N13" s="6" t="str">
+      <c r="N13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P13" s="3">
         <v>7</v>
-      </c>
-      <c r="P13" s="6">
-        <v>-1</v>
       </c>
       <c r="Q13" s="6">
         <v>-1</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S13" s="1">
         <v>107001</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>107002</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>107003</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <v>107004</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:2e7d958 commit_msg:Merge branch 'dev' of https://bitbucket.org/funplus/excel into dev ...
</commit_message>
<xml_diff>
--- a/config/excel/Hero.xlsx
+++ b/config/excel/Hero.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5380CE1-BEB8-4EF1-93A0-85CFB8FC3E1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowWidth="28125" windowHeight="12540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hero" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
@@ -123,9 +129,6 @@
     <t>quality</t>
   </si>
   <si>
-    <t>Profession</t>
-  </si>
-  <si>
     <t>race</t>
   </si>
   <si>
@@ -262,19 +265,33 @@
   </si>
   <si>
     <t>怪物3</t>
+  </si>
+  <si>
+    <t>profession</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>modelResource</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>模型资源</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="6" type="noConversion"/>
+  </si>
+  <si>
+    <t>puluomixiusi</t>
+    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="26">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -286,11 +303,13 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -307,163 +326,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Helvetica Neue"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Helvetica Neue"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="SimSun"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -494,194 +367,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="10">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -704,251 +391,9 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -971,57 +416,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -1094,6 +492,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -2164,16 +1565,16 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:U13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -2181,20 +1582,20 @@
     <col min="1" max="1" width="14.375" style="1" customWidth="1"/>
     <col min="2" max="2" width="13.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="17.375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.75" style="1" customWidth="1"/>
-    <col min="7" max="7" width="27.625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="16.25" style="1" customWidth="1"/>
-    <col min="10" max="13" width="9.375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="16.125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="16.75" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.5" style="1" customWidth="1"/>
-    <col min="17" max="17" width="20.125" style="1" customWidth="1"/>
-    <col min="18" max="21" width="9.25" style="1" customWidth="1"/>
-    <col min="22" max="16384" width="6" style="1"/>
+    <col min="4" max="6" width="17.375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="16.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="16.25" style="1" customWidth="1"/>
+    <col min="11" max="14" width="9.375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="16.125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="16.75" style="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="20.125" style="1" customWidth="1"/>
+    <col min="19" max="22" width="9.25" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.1" customHeight="1" spans="1:17">
+    <row r="1" spans="1:22" ht="14.1" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2214,63 +1615,67 @@
       <c r="O1" s="3"/>
       <c r="P1" s="3"/>
       <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
     </row>
-    <row r="2" ht="120.95" customHeight="1" spans="1:21">
+    <row r="2" spans="1:22" ht="120.95" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="L2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="4" t="s">
+      <c r="N2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="7" t="s">
+      <c r="O2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="8" t="s">
+      <c r="P2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
-      <c r="R2" s="9" t="s">
+      <c r="R2" s="2"/>
+      <c r="S2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="9" t="s">
+      <c r="T2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="T2" s="9" t="s">
+      <c r="U2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="U2" s="9" t="s">
+      <c r="V2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" ht="16.15" customHeight="1" spans="1:21">
+    <row r="3" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>17</v>
@@ -2282,120 +1687,126 @@
         <v>19</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="G3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="J3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J3" s="5"/>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
-      <c r="N3" s="5" t="s">
+      <c r="N3" s="5"/>
+      <c r="O3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="R3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q3" s="5" t="s">
+      <c r="S3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="R3" s="10" t="s">
+      <c r="T3" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="10" t="s">
+      <c r="U3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="T3" s="10" t="s">
+      <c r="V3" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="U3" s="10" t="s">
-        <v>32</v>
-      </c>
     </row>
-    <row r="4" ht="16.15" customHeight="1" spans="1:21">
+    <row r="4" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="G4" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="M4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="P4" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="O4" s="5" t="s">
+      <c r="Q4" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="P4" s="5" t="s">
+      <c r="R4" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q4" s="5" t="s">
+      <c r="S4" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="T4" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="S4" s="10" t="s">
+      <c r="U4" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="T4" s="10" t="s">
+      <c r="V4" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="U4" s="10" t="s">
-        <v>51</v>
-      </c>
     </row>
-    <row r="5" ht="16.15" customHeight="1" spans="1:21">
+    <row r="5" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -2410,86 +1821,90 @@
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
       <c r="Q5" s="5"/>
-      <c r="R5" s="10"/>
+      <c r="R5" s="5"/>
       <c r="S5" s="10"/>
       <c r="T5" s="10"/>
       <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
     </row>
-    <row r="6" ht="16.15" customHeight="1" spans="1:21">
+    <row r="6" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="D6" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="E6" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="G6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J6" s="5"/>
+        <v>54</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>54</v>
+      </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="5" t="s">
-        <v>58</v>
-      </c>
+      <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="P6" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q6" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="R6" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="V6" s="10" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="7" ht="24.95" customHeight="1" spans="1:21">
+    <row r="7" spans="1:22" ht="24.95" customHeight="1">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F7" s="6">
+      <c r="G7" s="6">
         <v>0</v>
       </c>
-      <c r="G7" s="6">
+      <c r="H7" s="6">
         <v>1</v>
-      </c>
-      <c r="H7" s="6">
-        <v>0</v>
       </c>
       <c r="I7" s="6">
         <v>0</v>
@@ -2506,52 +1921,55 @@
       <c r="M7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="6" t="str">
-        <f t="shared" ref="N7:N13" si="0">J7&amp;","&amp;K7&amp;","&amp;L7&amp;","&amp;M7</f>
+      <c r="N7" s="6">
+        <v>0</v>
+      </c>
+      <c r="O7" s="6" t="str">
+        <f t="shared" ref="O7:O13" si="0">K7&amp;","&amp;L7&amp;","&amp;M7&amp;","&amp;N7</f>
         <v>0,0,0,0</v>
       </c>
-      <c r="O7" s="6">
+      <c r="P7" s="6">
         <v>1</v>
       </c>
-      <c r="P7" s="6">
+      <c r="Q7" s="6">
         <v>50</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="R7" s="6">
         <v>30</v>
       </c>
-      <c r="R7" s="1">
+      <c r="S7" s="1">
         <v>101001</v>
       </c>
-      <c r="S7" s="1">
+      <c r="T7" s="1">
         <v>101002</v>
       </c>
-      <c r="T7" s="1">
+      <c r="U7" s="1">
         <v>101003</v>
       </c>
-      <c r="U7" s="1">
+      <c r="V7" s="1">
         <v>101004</v>
       </c>
     </row>
-    <row r="8" ht="24.95" customHeight="1" spans="1:21">
+    <row r="8" spans="1:22" ht="24.95" customHeight="1">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F8" s="6">
+      <c r="G8" s="6">
         <v>1</v>
       </c>
-      <c r="G8" s="6">
+      <c r="H8" s="6">
         <v>0</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1</v>
       </c>
       <c r="I8" s="6">
         <v>1</v>
@@ -2568,52 +1986,55 @@
       <c r="M8" s="6">
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="str">
+      <c r="N8" s="6">
+        <v>1</v>
+      </c>
+      <c r="O8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>1,1,1,1</v>
       </c>
-      <c r="O8" s="6">
+      <c r="P8" s="6">
         <v>2</v>
       </c>
-      <c r="P8" s="6">
+      <c r="Q8" s="6">
         <v>80</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>50</v>
       </c>
-      <c r="R8" s="1">
+      <c r="S8" s="1">
         <v>102001</v>
       </c>
-      <c r="S8" s="1">
+      <c r="T8" s="1">
         <v>102002</v>
       </c>
-      <c r="T8" s="1">
+      <c r="U8" s="1">
         <v>102003</v>
       </c>
-      <c r="U8" s="1">
+      <c r="V8" s="1">
         <v>102004</v>
       </c>
     </row>
-    <row r="9" ht="16.15" customHeight="1" spans="1:21">
+    <row r="9" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F9" s="3">
+        <v>72</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G9" s="3">
         <v>0</v>
       </c>
-      <c r="G9" s="3">
+      <c r="H9" s="3">
         <v>3</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2</v>
       </c>
       <c r="I9" s="3">
         <v>2</v>
@@ -2630,52 +2051,55 @@
       <c r="M9" s="3">
         <v>2</v>
       </c>
-      <c r="N9" s="6" t="str">
+      <c r="N9" s="3">
+        <v>2</v>
+      </c>
+      <c r="O9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>2,2,2,2</v>
       </c>
-      <c r="O9" s="3">
+      <c r="P9" s="3">
         <v>3</v>
       </c>
-      <c r="P9" s="6">
+      <c r="Q9" s="6">
         <v>50</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>30</v>
       </c>
-      <c r="R9" s="1">
+      <c r="S9" s="1">
         <v>103001</v>
       </c>
-      <c r="S9" s="1">
+      <c r="T9" s="1">
         <v>103002</v>
       </c>
-      <c r="T9" s="1">
+      <c r="U9" s="1">
         <v>103003</v>
       </c>
-      <c r="U9" s="1">
+      <c r="V9" s="1">
         <v>103004</v>
       </c>
     </row>
-    <row r="10" ht="14.1" customHeight="1" spans="1:21">
+    <row r="10" spans="1:22" ht="14.1" customHeight="1">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="3">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="3">
+      <c r="H10" s="3">
         <v>4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>3</v>
       </c>
       <c r="I10" s="3">
         <v>3</v>
@@ -2692,55 +2116,58 @@
       <c r="M10" s="3">
         <v>3</v>
       </c>
-      <c r="N10" s="6" t="str">
+      <c r="N10" s="3">
+        <v>3</v>
+      </c>
+      <c r="O10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>3,3,3,3</v>
       </c>
-      <c r="O10" s="3">
+      <c r="P10" s="3">
         <v>4</v>
       </c>
-      <c r="P10" s="6">
+      <c r="Q10" s="6">
         <v>80</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="R10" s="6">
         <v>50</v>
       </c>
-      <c r="R10" s="1">
+      <c r="S10" s="1">
         <v>104001</v>
       </c>
-      <c r="S10" s="1">
+      <c r="T10" s="1">
         <v>104002</v>
       </c>
-      <c r="T10" s="1">
+      <c r="U10" s="1">
         <v>104003</v>
       </c>
-      <c r="U10" s="1">
+      <c r="V10" s="1">
         <v>104004</v>
       </c>
     </row>
-    <row r="11" ht="24.95" customHeight="1" spans="1:21">
+    <row r="11" spans="1:22" ht="24.95" customHeight="1">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F11" s="6">
+        <v>72</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="6">
         <v>1</v>
       </c>
-      <c r="G11" s="6">
+      <c r="H11" s="6">
         <v>0</v>
       </c>
-      <c r="H11" s="6">
+      <c r="I11" s="6">
         <v>1</v>
-      </c>
-      <c r="I11" s="6">
-        <v>-1</v>
       </c>
       <c r="J11" s="6">
         <v>-1</v>
@@ -2754,55 +2181,58 @@
       <c r="M11" s="6">
         <v>-1</v>
       </c>
-      <c r="N11" s="6" t="str">
+      <c r="N11" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O11" s="6">
+      <c r="P11" s="6">
         <v>5</v>
-      </c>
-      <c r="P11" s="6">
-        <v>-1</v>
       </c>
       <c r="Q11" s="6">
         <v>-1</v>
       </c>
-      <c r="R11" s="1">
+      <c r="R11" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S11" s="1">
         <v>105001</v>
       </c>
-      <c r="S11" s="1">
+      <c r="T11" s="1">
         <v>105002</v>
       </c>
-      <c r="T11" s="1">
+      <c r="U11" s="1">
         <v>105003</v>
       </c>
-      <c r="U11" s="1">
+      <c r="V11" s="1">
         <v>105004</v>
       </c>
     </row>
-    <row r="12" ht="16.15" customHeight="1" spans="1:21">
+    <row r="12" spans="1:22" ht="16.149999999999999" customHeight="1">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="3">
+        <v>72</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G12" s="3">
         <v>0</v>
       </c>
-      <c r="G12" s="3">
+      <c r="H12" s="3">
         <v>3</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>2</v>
-      </c>
-      <c r="I12" s="6">
-        <v>-1</v>
       </c>
       <c r="J12" s="6">
         <v>-1</v>
@@ -2816,55 +2246,58 @@
       <c r="M12" s="6">
         <v>-1</v>
       </c>
-      <c r="N12" s="6" t="str">
+      <c r="N12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O12" s="3">
+      <c r="P12" s="3">
         <v>6</v>
-      </c>
-      <c r="P12" s="6">
-        <v>-1</v>
       </c>
       <c r="Q12" s="6">
         <v>-1</v>
       </c>
-      <c r="R12" s="1">
+      <c r="R12" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S12" s="1">
         <v>106001</v>
       </c>
-      <c r="S12" s="1">
+      <c r="T12" s="1">
         <v>106002</v>
       </c>
-      <c r="T12" s="1">
+      <c r="U12" s="1">
         <v>106003</v>
       </c>
-      <c r="U12" s="1">
+      <c r="V12" s="1">
         <v>106004</v>
       </c>
     </row>
-    <row r="13" ht="14.1" customHeight="1" spans="1:21">
+    <row r="13" spans="1:22" ht="14.1" customHeight="1">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="F13" s="3">
+        <v>72</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="G13" s="3">
+      <c r="H13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>3</v>
-      </c>
-      <c r="I13" s="6">
-        <v>-1</v>
       </c>
       <c r="J13" s="6">
         <v>-1</v>
@@ -2878,35 +2311,39 @@
       <c r="M13" s="6">
         <v>-1</v>
       </c>
-      <c r="N13" s="6" t="str">
+      <c r="N13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="O13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>-1,-1,-1,-1</v>
       </c>
-      <c r="O13" s="3">
+      <c r="P13" s="3">
         <v>7</v>
-      </c>
-      <c r="P13" s="6">
-        <v>-1</v>
       </c>
       <c r="Q13" s="6">
         <v>-1</v>
       </c>
-      <c r="R13" s="1">
+      <c r="R13" s="6">
+        <v>-1</v>
+      </c>
+      <c r="S13" s="1">
         <v>107001</v>
       </c>
-      <c r="S13" s="1">
+      <c r="T13" s="1">
         <v>107002</v>
       </c>
-      <c r="T13" s="1">
+      <c r="U13" s="1">
         <v>107003</v>
       </c>
-      <c r="U13" s="1">
+      <c r="V13" s="1">
         <v>107004</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
[excel-pipeline] hash_id:44e0139 commit_msg:增加初始怒气，修改英雄表批注 ...
</commit_message>
<xml_diff>
--- a/config/excel/Hero.xlsx
+++ b/config/excel/Hero.xlsx
@@ -1,31 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\EastEden\excel\global\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5380CE1-BEB8-4EF1-93A0-85CFB8FC3E1C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="24225" windowHeight="12540"/>
   </bookViews>
   <sheets>
     <sheet name="Hero" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>行列头两行不会被读取</t>
   </si>
   <si>
     <t>英雄和怪物id</t>
+  </si>
+  <si>
+    <t>模型资源</t>
   </si>
   <si>
     <t>单位米</t>
@@ -78,20 +75,9 @@
     <t>此列由前4列自动生成，不用填写</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">对应att表
+    <t xml:space="preserve">对应att表
 卡牌1级的属性固定值。
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="SimSun"/>
-        <charset val="134"/>
-      </rPr>
-      <t>demo版本目前临时填，正式后需要改成21</t>
-    </r>
   </si>
   <si>
     <t>Demo版本
@@ -123,12 +109,18 @@
     <t>name</t>
   </si>
   <si>
+    <t>modelResource</t>
+  </si>
+  <si>
     <t>modelscope</t>
   </si>
   <si>
     <t>quality</t>
   </si>
   <si>
+    <t>profession</t>
+  </si>
+  <si>
     <t>race</t>
   </si>
   <si>
@@ -240,6 +232,9 @@
     <t>demo版本防战</t>
   </si>
   <si>
+    <t>puluomixiusi</t>
+  </si>
+  <si>
     <t>1.5</t>
   </si>
   <si>
@@ -265,33 +260,19 @@
   </si>
   <si>
     <t>怪物3</t>
-  </si>
-  <si>
-    <t>profession</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>modelResource</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>模型资源</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>string</t>
-    <phoneticPr fontId="6" type="noConversion"/>
-  </si>
-  <si>
-    <t>puluomixiusi</t>
-    <phoneticPr fontId="6" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -303,13 +284,11 @@
       <sz val="9"/>
       <color indexed="8"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="微软雅黑"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
@@ -326,17 +305,157 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="SimSun"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="SimSun"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Helvetica Neue"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Helvetica Neue"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,8 +486,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -391,9 +696,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -416,10 +963,57 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
+    <cellStyle name="标题" xfId="17" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="计算" xfId="25" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
+    <cellStyle name="汇总" xfId="30" builtinId="25"/>
+    <cellStyle name="好" xfId="31" builtinId="26"/>
+    <cellStyle name="适中" xfId="32" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
@@ -492,9 +1086,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1565,16 +2156,16 @@
       </a:style>
     </a:txDef>
   </a:objectDefaults>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:V13"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="13.35" customHeight="1"/>
@@ -1595,7 +2186,7 @@
     <col min="23" max="16384" width="6" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="14.1" customHeight="1">
+    <row r="1" ht="14.1" customHeight="1" spans="1:18">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1617,7 +2208,7 @@
       <c r="Q1" s="3"/>
       <c r="R1" s="3"/>
     </row>
-    <row r="2" spans="1:22" ht="120.95" customHeight="1">
+    <row r="2" ht="120.95" customHeight="1" spans="1:22">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="2" t="s">
@@ -1625,188 +2216,188 @@
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="P2" s="8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
       <c r="S2" s="9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="U2" s="9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V2" s="9" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="3" ht="16.15" customHeight="1" spans="1:22">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>69</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K3" s="5"/>
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="S3" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T3" s="10" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="U3" s="10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="V3" s="10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="4" ht="16.15" customHeight="1" spans="1:22">
       <c r="A4" s="3"/>
       <c r="B4" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="K4" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="M4" s="5" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="N4" s="5" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="5" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="S4" s="10" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="T4" s="10" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="U4" s="10" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="V4" s="10" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="5" ht="16.15" customHeight="1" spans="1:22">
       <c r="A5" s="3"/>
       <c r="B5" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -1827,78 +2418,78 @@
       <c r="U5" s="10"/>
       <c r="V5" s="10"/>
     </row>
-    <row r="6" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="6" ht="16.15" customHeight="1" spans="1:22">
       <c r="A6" s="3"/>
       <c r="B6" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="Q6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="S6" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="U6" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="V6" s="10" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="24.95" customHeight="1">
+    <row r="7" ht="24.95" customHeight="1" spans="1:22">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G7" s="6">
         <v>0</v>
@@ -1950,20 +2541,20 @@
         <v>101004</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="24.95" customHeight="1">
+    <row r="8" ht="24.95" customHeight="1" spans="1:22">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="6">
         <v>2</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G8" s="6">
         <v>1</v>
@@ -2015,20 +2606,20 @@
         <v>102004</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="9" ht="16.15" customHeight="1" spans="1:22">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="6">
         <v>3</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>72</v>
-      </c>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G9" s="3">
         <v>0</v>
@@ -2080,20 +2671,20 @@
         <v>103004</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="14.1" customHeight="1">
+    <row r="10" ht="14.1" customHeight="1" spans="1:22">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="6">
         <v>4</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="G10" s="3">
         <v>1</v>
@@ -2145,20 +2736,20 @@
         <v>104004</v>
       </c>
     </row>
-    <row r="11" spans="1:22" ht="24.95" customHeight="1">
+    <row r="11" ht="24.95" customHeight="1" spans="1:22">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="6">
         <v>5</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>61</v>
       </c>
       <c r="G11" s="6">
         <v>1</v>
@@ -2210,20 +2801,20 @@
         <v>105004</v>
       </c>
     </row>
-    <row r="12" spans="1:22" ht="16.149999999999999" customHeight="1">
+    <row r="12" ht="16.15" customHeight="1" spans="1:22">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="6">
         <v>6</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G12" s="3">
         <v>0</v>
@@ -2275,20 +2866,20 @@
         <v>106004</v>
       </c>
     </row>
-    <row r="13" spans="1:22" ht="14.1" customHeight="1">
+    <row r="13" ht="14.1" customHeight="1" spans="1:22">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="6">
         <v>7</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G13" s="3">
         <v>1</v>
@@ -2341,9 +2932,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" useFirstPageNumber="1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="portrait" useFirstPageNumber="1"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>